<commit_message>
* Added in Lengths file * Updates to payload files to take into account increased size in Tray * Fixed airframe which had holes in wrong spot.
</commit_message>
<xml_diff>
--- a/DraftDrawings/Payload/Lengths.xlsx
+++ b/DraftDrawings/Payload/Lengths.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
   <si>
     <t>Coupler</t>
   </si>
@@ -76,6 +76,9 @@
   </si>
   <si>
     <t>Component</t>
+  </si>
+  <si>
+    <t>Phenolic tube density (g/m)</t>
   </si>
 </sst>
 </file>
@@ -119,9 +122,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -423,10 +427,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:D23"/>
+  <dimension ref="A2:D24"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -588,11 +592,11 @@
         <v>8</v>
       </c>
       <c r="B14">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C14">
         <f>B14</f>
-        <v>90</v>
+        <v>92</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -622,7 +626,7 @@
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C18">
         <f>SUM(C3:C16)</f>
-        <v>308</v>
+        <v>310</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -634,7 +638,15 @@
       </c>
       <c r="C23">
         <f>C18/1000*B23</f>
-        <v>100.408</v>
+        <v>101.06</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B24" s="2">
+        <v>203</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
* Created Disc and Phenolic Spacer * Reduced length of airframe back to 310mm (removed space 2 x 2mm in inter-mount) * Added 'centre' crosshairs in drill holes on other drawings to aid in transferring to wood.
</commit_message>
<xml_diff>
--- a/DraftDrawings/Payload/Lengths.xlsx
+++ b/DraftDrawings/Payload/Lengths.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
   <si>
     <t>Coupler</t>
   </si>
@@ -60,18 +60,12 @@
     <t>Notes</t>
   </si>
   <si>
-    <t>Interchange upper/lower connectors WITHIN interchange. These are each 6mm thick</t>
-  </si>
-  <si>
     <t>Height</t>
   </si>
   <si>
     <t>Contribution to height of airframe</t>
   </si>
   <si>
-    <t>Intermount upper/lower connectors WITHIN intermount. These are each 6mm thick</t>
-  </si>
-  <si>
     <t>Quantum Tube Density (g/m)</t>
   </si>
   <si>
@@ -79,6 +73,106 @@
   </si>
   <si>
     <t>Phenolic tube density (g/m)</t>
+  </si>
+  <si>
+    <t>Plywood disc component that has the Stepper motor mounted to</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Phenolic Tube that has </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>s2 mount</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>s2 inter-mount</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> installed in it</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Phenolic Tube that has </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>s1 mount</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>s1 inter-mount</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> installed in it</t>
+    </r>
+  </si>
+  <si>
+    <t>Phenolic tube that has interchange-lower at bottom and interchange-upper in it.</t>
   </si>
 </sst>
 </file>
@@ -429,8 +523,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:D24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -441,13 +535,13 @@
   <sheetData>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>16</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>13</v>
@@ -474,21 +568,23 @@
       <c r="C4">
         <v>0</v>
       </c>
+      <c r="D4" s="2" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>11</v>
       </c>
       <c r="B5">
-        <f>25+B4+B6</f>
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C5">
         <f>B5</f>
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D5" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -518,12 +614,14 @@
         <v>11</v>
       </c>
       <c r="B8">
-        <f>25+B7+B9</f>
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C8">
         <f>B8</f>
-        <v>37</v>
+        <v>35</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -537,6 +635,9 @@
         <f>0</f>
         <v>0</v>
       </c>
+      <c r="D9" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -561,7 +662,7 @@
         <v>30</v>
       </c>
       <c r="D11" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -580,11 +681,11 @@
         <v>7</v>
       </c>
       <c r="B13">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C13">
         <f>B13</f>
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -604,11 +705,11 @@
         <v>9</v>
       </c>
       <c r="B15">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C15">
         <f>B15</f>
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -631,7 +732,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B23">
         <v>326</v>
@@ -643,7 +744,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B24" s="2">
         <v>203</v>

</xml_diff>

<commit_message>
* Correct positioning of holes in Air Frame * More information added to Lengths.xlsx * Other minor updates
</commit_message>
<xml_diff>
--- a/DraftDrawings/Payload/Lengths.xlsx
+++ b/DraftDrawings/Payload/Lengths.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="30">
   <si>
     <t>Coupler</t>
   </si>
@@ -24,12 +24,6 @@
     <t>s2 mount</t>
   </si>
   <si>
-    <t>s2 inter-mount</t>
-  </si>
-  <si>
-    <t>s1 inter-mount</t>
-  </si>
-  <si>
     <t>s1 mount</t>
   </si>
   <si>
@@ -49,9 +43,6 @@
   </si>
   <si>
     <t>Nose Cone</t>
-  </si>
-  <si>
-    <t>inter-mount</t>
   </si>
   <si>
     <t>interchange</t>
@@ -173,6 +164,36 @@
   </si>
   <si>
     <t>Phenolic tube that has interchange-lower at bottom and interchange-upper in it.</t>
+  </si>
+  <si>
+    <t>s2 inter-mount Disc</t>
+  </si>
+  <si>
+    <t>s1 inter-mount Disc</t>
+  </si>
+  <si>
+    <t>Tube inter-mount</t>
+  </si>
+  <si>
+    <t>Part</t>
+  </si>
+  <si>
+    <t>Coupler Tube</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S2 </t>
+  </si>
+  <si>
+    <t>S1</t>
+  </si>
+  <si>
+    <t>S1-Elect</t>
+  </si>
+  <si>
+    <t>Elect</t>
+  </si>
+  <si>
+    <t>THESE VALUES ARE GOING TO CHANGE!</t>
   </si>
 </sst>
 </file>
@@ -521,232 +542,259 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:D24"/>
+  <dimension ref="A2:E24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3">
+        <v>90</v>
+      </c>
+      <c r="D3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>6</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5">
+        <v>35</v>
+      </c>
+      <c r="D5">
+        <f>C5</f>
+        <v>35</v>
+      </c>
+      <c r="E5" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6">
+        <v>6</v>
+      </c>
+      <c r="D6">
         <v>0</v>
       </c>
-      <c r="B3">
-        <v>90</v>
-      </c>
-      <c r="C3">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4">
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7">
         <v>6</v>
       </c>
-      <c r="C4">
+      <c r="D7">
         <v>0</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5">
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8">
         <v>35</v>
       </c>
-      <c r="C5">
-        <f>B5</f>
+      <c r="D8">
+        <f>C8</f>
         <v>35</v>
       </c>
-      <c r="D5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="E8" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
         <v>2</v>
       </c>
-      <c r="B6">
+      <c r="C9">
         <v>6</v>
       </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7">
-        <v>6</v>
-      </c>
-      <c r="C7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8">
-        <v>35</v>
-      </c>
-      <c r="C8">
-        <f>B8</f>
-        <v>35</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>4</v>
-      </c>
-      <c r="B9">
-        <v>6</v>
-      </c>
-      <c r="C9">
+      <c r="D9">
         <f>0</f>
         <v>0</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10">
+        <v>6</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11">
+        <v>30</v>
+      </c>
+      <c r="D11">
+        <f>C11</f>
+        <v>30</v>
+      </c>
+      <c r="E11" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12">
+        <v>6</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" t="s">
         <v>5</v>
       </c>
-      <c r="B10">
+      <c r="C13">
+        <v>9</v>
+      </c>
+      <c r="D13">
+        <f>C13</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
         <v>6</v>
       </c>
-      <c r="C10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11">
-        <v>30</v>
-      </c>
-      <c r="C11">
-        <f>B11</f>
-        <v>30</v>
-      </c>
-      <c r="D11" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>6</v>
-      </c>
-      <c r="B12">
-        <v>6</v>
-      </c>
-      <c r="C12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="C14">
+        <v>92</v>
+      </c>
+      <c r="D14">
+        <f>C14</f>
+        <v>92</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
         <v>7</v>
       </c>
-      <c r="B13">
+      <c r="C15">
         <v>9</v>
       </c>
-      <c r="C13">
-        <f>B13</f>
+      <c r="D15">
+        <f>C15</f>
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B14">
-        <v>92</v>
-      </c>
-      <c r="C14">
-        <f>B14</f>
-        <v>92</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>9</v>
-      </c>
-      <c r="B15">
-        <v>9</v>
-      </c>
-      <c r="C15">
-        <f>B15</f>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>10</v>
-      </c>
-      <c r="B16">
+      <c r="B16" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16">
         <v>60</v>
       </c>
-      <c r="C16">
-        <f>B16</f>
+      <c r="D16">
+        <f>C16</f>
         <v>60</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C18">
-        <f>SUM(C3:C16)</f>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D18">
+        <f>SUM(D3:D16)</f>
         <v>310</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>16</v>
-      </c>
-      <c r="B23">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>13</v>
+      </c>
+      <c r="C23">
         <v>326</v>
       </c>
-      <c r="C23">
-        <f>C18/1000*B23</f>
+      <c r="D23">
+        <f>D18/1000*C23</f>
         <v>101.06</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B24" s="2">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B24" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C24" s="2">
         <v>203</v>
       </c>
     </row>

</xml_diff>

<commit_message>
* Created camera tray components
</commit_message>
<xml_diff>
--- a/DraftDrawings/Payload/Lengths.xlsx
+++ b/DraftDrawings/Payload/Lengths.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="90" windowWidth="18195" windowHeight="6975"/>
+    <workbookView xWindow="360" yWindow="90" windowWidth="18195" windowHeight="6975" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="KATE" sheetId="1" r:id="rId1"/>
+    <sheet name="CAMERA" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="38">
   <si>
     <t>Coupler</t>
   </si>
@@ -194,6 +194,30 @@
   </si>
   <si>
     <t>THESE VALUES ARE GOING TO CHANGE!</t>
+  </si>
+  <si>
+    <t>Bottom-Disc</t>
+  </si>
+  <si>
+    <t>Tray</t>
+  </si>
+  <si>
+    <t>Top Disc</t>
+  </si>
+  <si>
+    <t>Slides down within the coupler tube</t>
+  </si>
+  <si>
+    <t>Has the camera fixed to this</t>
+  </si>
+  <si>
+    <t>Sits above the coupler. Had 24 + 6 = 30mm of Phenolic Tube (which is fixed to the airframe using rivets)</t>
+  </si>
+  <si>
+    <t>Electronics</t>
+  </si>
+  <si>
+    <t>Camera Mount Platform</t>
   </si>
 </sst>
 </file>
@@ -544,8 +568,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:E24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -806,12 +830,231 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="36" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="2">
+        <v>90</v>
+      </c>
+      <c r="D2" s="2">
+        <v>40</v>
+      </c>
+      <c r="E2" s="2"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="2">
+        <v>6</v>
+      </c>
+      <c r="D3" s="2">
+        <v>0</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" s="2">
+        <v>77</v>
+      </c>
+      <c r="D4" s="2">
+        <v>24</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="2">
+        <v>6</v>
+      </c>
+      <c r="D5" s="2">
+        <v>6</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="2">
+        <v>9</v>
+      </c>
+      <c r="D6" s="2">
+        <f>C6</f>
+        <v>9</v>
+      </c>
+      <c r="E6" s="2"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="2">
+        <v>92</v>
+      </c>
+      <c r="D7" s="2">
+        <f>C7</f>
+        <v>92</v>
+      </c>
+      <c r="E7" s="2"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="2">
+        <v>9</v>
+      </c>
+      <c r="D8" s="2">
+        <f>C8</f>
+        <v>9</v>
+      </c>
+      <c r="E8" s="2"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="2">
+        <v>60</v>
+      </c>
+      <c r="D9" s="2">
+        <f>C9</f>
+        <v>60</v>
+      </c>
+      <c r="E9" s="2"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2">
+        <f>SUM(D2:D9)</f>
+        <v>240</v>
+      </c>
+      <c r="E11" s="2"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="2"/>
+      <c r="B16" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="2">
+        <v>326</v>
+      </c>
+      <c r="D16" s="2">
+        <f>D11/1000*C16</f>
+        <v>78.239999999999995</v>
+      </c>
+      <c r="E16" s="2"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="2"/>
+      <c r="B17" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" s="2">
+        <v>203</v>
+      </c>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
* Fixed up airframe by moving text into correct areas * Cleaning up dimensions * Moved the two wire exit holes to 59 and 55mm from top of payload airframe.
</commit_message>
<xml_diff>
--- a/DraftDrawings/Payload/Lengths.xlsx
+++ b/DraftDrawings/Payload/Lengths.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="90" windowWidth="18195" windowHeight="6975" activeTab="1"/>
@@ -11,12 +11,12 @@
     <sheet name="CAMERA" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="45">
   <si>
     <t>Coupler</t>
   </si>
@@ -219,6 +219,27 @@
   <si>
     <t>Camera Mount Platform</t>
   </si>
+  <si>
+    <t>TOTAL</t>
+  </si>
+  <si>
+    <t>Screws</t>
+  </si>
+  <si>
+    <t>Phenolic adaptor</t>
+  </si>
+  <si>
+    <t>Air Frame</t>
+  </si>
+  <si>
+    <t>Airframe</t>
+  </si>
+  <si>
+    <t>Mass (grams)</t>
+  </si>
+  <si>
+    <t>Camera</t>
+  </si>
 </sst>
 </file>
 
@@ -241,12 +262,30 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -261,10 +300,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -830,10 +875,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -841,221 +886,365 @@
     <col min="1" max="1" width="36" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="31.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.7109375" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="2" t="s">
+    <row r="2" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" s="4">
+        <v>240</v>
+      </c>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4">
+        <v>78</v>
+      </c>
+      <c r="F2" s="1"/>
+    </row>
+    <row r="3" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="1"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C4" s="5">
         <v>90</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D4" s="5">
         <v>40</v>
       </c>
-      <c r="E2" s="2"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="E4" s="5">
+        <v>18</v>
+      </c>
+      <c r="F4" s="2"/>
+    </row>
+    <row r="5" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="5"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B6" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C6" s="7">
         <v>6</v>
       </c>
-      <c r="D3" s="2">
-        <v>0</v>
-      </c>
-      <c r="E3" s="2" t="s">
+      <c r="D6" s="7">
+        <v>0</v>
+      </c>
+      <c r="E6" s="7">
+        <v>10</v>
+      </c>
+      <c r="F6" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2" t="s">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="7"/>
+      <c r="B7" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C7" s="7">
         <v>77</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D7" s="7">
         <v>24</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E7" s="7">
+        <v>15</v>
+      </c>
+      <c r="F7" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2" t="s">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="7"/>
+      <c r="B8" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C8" s="7">
         <v>6</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D8" s="7">
         <v>6</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E8" s="7">
+        <v>10</v>
+      </c>
+      <c r="F8" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+    <row r="9" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="7"/>
+      <c r="B9" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9" s="7">
+        <v>0</v>
+      </c>
+      <c r="D9" s="7">
+        <v>0</v>
+      </c>
+      <c r="E9" s="7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="7"/>
+      <c r="B10" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C10" s="7">
+        <v>0</v>
+      </c>
+      <c r="D10" s="7">
+        <v>0</v>
+      </c>
+      <c r="E10" s="7">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="7"/>
+      <c r="B11" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="C11" s="7">
+        <v>60</v>
+      </c>
+      <c r="D11" s="7">
+        <v>0</v>
+      </c>
+      <c r="E11" s="7">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="7"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+    </row>
+    <row r="13" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="7"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B14" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C14" s="5">
         <v>9</v>
       </c>
-      <c r="D6" s="2">
-        <f>C6</f>
+      <c r="D14" s="5">
+        <f>C14</f>
         <v>9</v>
       </c>
-      <c r="E6" s="2"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2" t="s">
+      <c r="E14" s="5">
+        <v>10</v>
+      </c>
+      <c r="F14" s="2"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="5"/>
+      <c r="B15" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C15" s="5">
         <v>92</v>
       </c>
-      <c r="D7" s="2">
-        <f>C7</f>
+      <c r="D15" s="5">
+        <f>C15</f>
         <v>92</v>
       </c>
-      <c r="E7" s="2"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2" t="s">
+      <c r="E15" s="5">
+        <v>14</v>
+      </c>
+      <c r="F15" s="2"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="5"/>
+      <c r="B16" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C16" s="5">
         <v>9</v>
       </c>
-      <c r="D8" s="2">
-        <f>C8</f>
+      <c r="D16" s="5">
+        <f>C16</f>
         <v>9</v>
       </c>
-      <c r="E8" s="2"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+      <c r="E16" s="5">
+        <v>10</v>
+      </c>
+      <c r="F16" s="2"/>
+    </row>
+    <row r="17" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="5"/>
+      <c r="B17" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17" s="5">
+        <v>0</v>
+      </c>
+      <c r="D17" s="5">
+        <v>0</v>
+      </c>
+      <c r="E17" s="5">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="5"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B19" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C19" s="7">
         <v>60</v>
       </c>
-      <c r="D9" s="2">
-        <f>C9</f>
+      <c r="D19" s="7">
+        <f>C19</f>
         <v>60</v>
       </c>
-      <c r="E9" s="2"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2">
-        <f>SUM(D2:D9)</f>
+      <c r="E19" s="7"/>
+      <c r="F19" s="2"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="7"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="2"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F21" s="2"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F22" s="2"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F23" s="2"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="2"/>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="F24" s="2"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="2"/>
+      <c r="B25" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2">
+        <f>SUM(D2:D19)</f>
         <v>240</v>
       </c>
-      <c r="E11" s="2"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
+      <c r="E25" s="2">
+        <f>SUM(E2:E20)</f>
+        <v>287</v>
+      </c>
+      <c r="F25" s="2"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="2"/>
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="F26" s="2"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="2"/>
-      <c r="B16" s="2" t="s">
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="F27" s="2"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B32" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="2">
+      <c r="C32" s="2">
         <v>326</v>
       </c>
-      <c r="D16" s="2">
-        <f>D11/1000*C16</f>
+      <c r="D32" s="2">
+        <f>D25/1000*C32</f>
         <v>78.239999999999995</v>
       </c>
-      <c r="E16" s="2"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="2"/>
-      <c r="B17" s="2" t="s">
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B33" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="2">
+      <c r="C33" s="2">
         <v>203</v>
       </c>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
+      <c r="D33" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>